<commit_message>
add API: create or update set
</commit_message>
<xml_diff>
--- a/DOC/API list.xlsx
+++ b/DOC/API list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\flashcard\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285714AE-9DCF-421B-8F52-E813373E4B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1CC03F-FF25-4AC8-8439-DC126D5DACDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -75,79 +75,89 @@
 # password</t>
   </si>
   <si>
-    <t>CreateSet</t>
+    <t>CreateFolder</t>
+  </si>
+  <si>
+    <t>Tạo folder hoặc update folder
+nếu truyền folder ID thì là update còn 0 là tạo mới</t>
+  </si>
+  <si>
+    <t>tạo set và cập nhật set
+nếu truyền setID thì là update còn 0 là tạo mới</t>
+  </si>
+  <si>
+    <t># tên folder
+# mô tả folder</t>
+  </si>
+  <si>
+    <t>recentSets</t>
+  </si>
+  <si>
+    <t>Trả về list set học gần đây</t>
+  </si>
+  <si>
+    <t>trả về thông tin của set và % đã học thuộc</t>
+  </si>
+  <si>
+    <t>trả về thông tin folder cùng các set của nó</t>
+  </si>
+  <si>
+    <t>listFolders</t>
+  </si>
+  <si>
+    <t>SetToFolder</t>
+  </si>
+  <si>
+    <t>thêm set tự do vào folder</t>
+  </si>
+  <si>
+    <t># setID
+# folderID</t>
+  </si>
+  <si>
+    <t>deleteSet</t>
+  </si>
+  <si>
+    <t>deleteFolder</t>
+  </si>
+  <si>
+    <t>Xóa 1 set</t>
+  </si>
+  <si>
+    <t>Xóa 1 folder</t>
+  </si>
+  <si>
+    <t># folderID</t>
+  </si>
+  <si>
+    <t># setID</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
   <si>
     <t># setID( 0 hoặc khác 0)
 # tên set
-# mô tả set
+# giá tiền
 # folder ID( bằng 0 nếu ko thuộc folder nào hoặc khác 0)
-# cards : [{front, back}, {front, back}, ...]</t>
-  </si>
-  <si>
-    <t>CreateFolder</t>
-  </si>
-  <si>
-    <t>Tạo folder hoặc update folder
-nếu truyền folder ID thì là update còn 0 là tạo mới</t>
-  </si>
-  <si>
-    <t>tạo set và cập nhật set
-nếu truyền setID thì là update còn 0 là tạo mới</t>
-  </si>
-  <si>
-    <t># tên folder
-# mô tả folder</t>
-  </si>
-  <si>
-    <t>recentSets</t>
-  </si>
-  <si>
-    <t>Trả về list set học gần đây</t>
-  </si>
-  <si>
-    <t>trả về thông tin của set và % đã học thuộc</t>
-  </si>
-  <si>
-    <t>trả về thông tin folder cùng các set của nó</t>
-  </si>
-  <si>
-    <t>listFolders</t>
-  </si>
-  <si>
-    <t>SetToFolder</t>
-  </si>
-  <si>
-    <t>thêm set tự do vào folder</t>
-  </si>
-  <si>
-    <t># setID
-# folderID</t>
-  </si>
-  <si>
-    <t>deleteSet</t>
-  </si>
-  <si>
-    <t>deleteFolder</t>
-  </si>
-  <si>
-    <t>Xóa 1 set</t>
-  </si>
-  <si>
-    <t>Xóa 1 folder</t>
-  </si>
-  <si>
-    <t># folderID</t>
-  </si>
-  <si>
-    <t># setID</t>
+#card ID (bằng 0 nếu là card mới thêm, khác 0 nếu sửa)
+# cards : [{'id': x, front': value1, 'back' : value2}, {…..}, ...]</t>
+  </si>
+  <si>
+    <t>createOrUpdateSet</t>
+  </si>
+  <si>
+    <t>Hiện tại đang trả về 5 cái và fake % đã học</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +188,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF00B050"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFF0000"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -205,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +263,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,9 +565,10 @@
     <col min="2" max="2" width="32.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="94.90625" style="2" customWidth="1"/>
     <col min="4" max="5" width="65.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="45.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -544,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="9" customFormat="1" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -560,9 +604,11 @@
       <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" ht="37" x14ac:dyDescent="0.35">
+      <c r="F3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="9" customFormat="1" ht="37" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -578,9 +624,11 @@
       <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F4" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -592,119 +640,134 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="92.5" x14ac:dyDescent="0.35">
+      <c r="F5" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="150.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="37" x14ac:dyDescent="0.35">
+      <c r="F6" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="37" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" ht="37" x14ac:dyDescent="0.35">
+      <c r="F9" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="9" customFormat="1" ht="37" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F11" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -712,9 +775,9 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -722,9 +785,9 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -732,9 +795,9 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -742,9 +805,9 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -752,7 +815,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
@@ -762,7 +825,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
@@ -772,7 +835,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
@@ -782,7 +845,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
@@ -792,7 +855,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
@@ -802,7 +865,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
@@ -812,7 +875,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
@@ -822,7 +885,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>